<commit_message>
Update list of websites
</commit_message>
<xml_diff>
--- a/psse komunikaty.xlsx
+++ b/psse komunikaty.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\covid_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DDD7B5-DB9B-4CBB-8B86-69380CDBF762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618B288D-A483-4F7B-9D3A-6CA5FCA1FFA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECA93252-637E-4118-864B-BDBC199DBE52}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="419">
   <si>
     <t>powiat</t>
   </si>
@@ -1251,6 +1251,48 @@
   </si>
   <si>
     <t>https://sanepid.nidzica.pl/koronawirus</t>
+  </si>
+  <si>
+    <t>http://plock.psse.waw.pl/aktualnosci-i-komunikaty-6796/komunikaty</t>
+  </si>
+  <si>
+    <t>http://wolomin.psse.waw.pl/1365</t>
+  </si>
+  <si>
+    <t>brak</t>
+  </si>
+  <si>
+    <t>https://www.psse.bielsko.pl/</t>
+  </si>
+  <si>
+    <t>http://www.psse.pajeczno.com/index.php?p=p5</t>
+  </si>
+  <si>
+    <t>https://www.pssedg.pl/</t>
+  </si>
+  <si>
+    <t>http://www.bip.visacom.pl/psse_elk/</t>
+  </si>
+  <si>
+    <t>http://www.psseopatow.pl/</t>
+  </si>
+  <si>
+    <t>http://psse.czest.pl/koronawirus-dane.html</t>
+  </si>
+  <si>
+    <t>http://psse-zawiercie.internetdsl.pl/</t>
+  </si>
+  <si>
+    <t>http://psseluban.pl/</t>
+  </si>
+  <si>
+    <t>http://www.psse-gostyn.pl/</t>
+  </si>
+  <si>
+    <t>http://www.psse-konin.pl/koronawirus-2019-ncov</t>
+  </si>
+  <si>
+    <t>http://www.psse-poznan.pl/p,169,covid-19-dane-statystyczne</t>
   </si>
 </sst>
 </file>
@@ -1605,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA135E91-B103-4B08-9F13-85FC983BFCF7}">
   <dimension ref="A1:E381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="B180" sqref="B180"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="D236" sqref="D236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,6 +1735,9 @@
       <c r="C6" t="s">
         <v>386</v>
       </c>
+      <c r="D6" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1781,6 +1826,9 @@
       <c r="C14" t="s">
         <v>386</v>
       </c>
+      <c r="D14" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1792,6 +1840,9 @@
       <c r="C15" t="s">
         <v>386</v>
       </c>
+      <c r="D15" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1919,6 +1970,9 @@
       <c r="C26" t="s">
         <v>383</v>
       </c>
+      <c r="D26" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1930,6 +1984,9 @@
       <c r="C27" t="s">
         <v>387</v>
       </c>
+      <c r="D27" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2068,6 +2125,9 @@
       <c r="C39" t="s">
         <v>380</v>
       </c>
+      <c r="D39" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -2112,6 +2172,9 @@
       <c r="C43" t="s">
         <v>386</v>
       </c>
+      <c r="D43" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -2123,6 +2186,9 @@
       <c r="C44" t="s">
         <v>386</v>
       </c>
+      <c r="D44" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -2148,6 +2214,9 @@
       <c r="C46" t="s">
         <v>386</v>
       </c>
+      <c r="D46" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -2236,6 +2305,9 @@
       <c r="C54" t="s">
         <v>388</v>
       </c>
+      <c r="D54" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -2365,7 +2437,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>357</v>
       </c>
@@ -2376,7 +2448,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -2387,7 +2459,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>318</v>
       </c>
@@ -2398,7 +2470,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>121</v>
       </c>
@@ -2409,7 +2481,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -2420,7 +2492,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>92</v>
       </c>
@@ -2431,7 +2503,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>142</v>
       </c>
@@ -2442,7 +2514,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>325</v>
       </c>
@@ -2452,8 +2524,11 @@
       <c r="C72" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -2464,7 +2539,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>219</v>
       </c>
@@ -2475,7 +2550,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>143</v>
       </c>
@@ -2486,7 +2561,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>143</v>
       </c>
@@ -2497,7 +2572,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>144</v>
       </c>
@@ -2508,7 +2583,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>54</v>
       </c>
@@ -2519,7 +2594,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>39</v>
       </c>
@@ -2530,7 +2605,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>358</v>
       </c>
@@ -2541,7 +2616,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>359</v>
       </c>
@@ -2552,7 +2627,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>220</v>
       </c>
@@ -2563,7 +2638,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>60</v>
       </c>
@@ -2574,7 +2649,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>307</v>
       </c>
@@ -2585,7 +2660,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>40</v>
       </c>
@@ -2595,8 +2670,11 @@
       <c r="C85" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>61</v>
       </c>
@@ -2607,7 +2685,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>326</v>
       </c>
@@ -2618,7 +2696,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>195</v>
       </c>
@@ -2629,7 +2707,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -2640,7 +2718,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>274</v>
       </c>
@@ -2651,7 +2729,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -2662,7 +2740,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>275</v>
       </c>
@@ -2673,7 +2751,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>29</v>
       </c>
@@ -2684,7 +2762,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -2695,7 +2773,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>288</v>
       </c>
@@ -2706,7 +2784,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>327</v>
       </c>
@@ -2796,6 +2874,9 @@
       <c r="C103" t="s">
         <v>382</v>
       </c>
+      <c r="D103" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
@@ -2807,6 +2888,9 @@
       <c r="C104" t="s">
         <v>389</v>
       </c>
+      <c r="D104" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
@@ -2939,6 +3023,9 @@
       <c r="C116" t="s">
         <v>389</v>
       </c>
+      <c r="D116" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
@@ -2950,6 +3037,9 @@
       <c r="C117" t="s">
         <v>389</v>
       </c>
+      <c r="D117" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
@@ -3169,6 +3259,9 @@
       <c r="C135" t="s">
         <v>375</v>
       </c>
+      <c r="D135" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
@@ -3180,6 +3273,9 @@
       <c r="C136" t="s">
         <v>375</v>
       </c>
+      <c r="D136" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
@@ -3304,6 +3400,9 @@
       <c r="C147" t="s">
         <v>375</v>
       </c>
+      <c r="D147" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
@@ -3838,6 +3937,9 @@
       <c r="C192" t="s">
         <v>380</v>
       </c>
+      <c r="D192" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
@@ -3970,6 +4072,9 @@
       <c r="C204" t="s">
         <v>387</v>
       </c>
+      <c r="D204" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
@@ -4151,7 +4256,7 @@
         <v>402</v>
       </c>
       <c r="E219" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -4275,6 +4380,9 @@
       <c r="C229" t="s">
         <v>381</v>
       </c>
+      <c r="D229" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
@@ -4286,6 +4394,9 @@
       <c r="C230" t="s">
         <v>381</v>
       </c>
+      <c r="D230" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
@@ -4347,6 +4458,9 @@
       <c r="C235" t="s">
         <v>389</v>
       </c>
+      <c r="D235" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
@@ -4358,6 +4472,9 @@
       <c r="C236" t="s">
         <v>389</v>
       </c>
+      <c r="D236" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
@@ -5168,6 +5285,9 @@
       <c r="C305" t="s">
         <v>388</v>
       </c>
+      <c r="D305" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
@@ -5505,6 +5625,9 @@
       <c r="C334" t="s">
         <v>375</v>
       </c>
+      <c r="D334" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
@@ -5516,6 +5639,9 @@
       <c r="C335" t="s">
         <v>375</v>
       </c>
+      <c r="D335" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
@@ -5729,6 +5855,9 @@
       <c r="C353" t="s">
         <v>381</v>
       </c>
+      <c r="D353" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
@@ -5861,6 +5990,9 @@
       <c r="C365" t="s">
         <v>386</v>
       </c>
+      <c r="D365" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
@@ -5871,9 +6003,6 @@
       </c>
       <c r="C366" t="s">
         <v>375</v>
-      </c>
-      <c r="D366" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>